<commit_message>
Finished Political Affilications Dashboard. Further updated Airport Dashboard. Started new dashboards for General Covid Stats for my storyboard introduction.
</commit_message>
<xml_diff>
--- a/Time Log for CISC 4900.xlsx
+++ b/Time Log for CISC 4900.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="916 - 930" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="101 - 1014" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="1015 - 1028" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="1029 - 1112" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'101 - 1014'!$A$1:$E$15</definedName>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
   <si>
     <t>DATE</t>
   </si>
@@ -305,6 +306,48 @@
   <si>
     <t>Worked on presentation slides</t>
   </si>
+  <si>
+    <t>looked for ways to contain Alaska and Hawaii in seperate containers and still be able to use them as filters</t>
+  </si>
+  <si>
+    <t>Built upon the Covid 2020 Death Report. It now includes Infection as well. Modernized the design of that dashboard as well.</t>
+  </si>
+  <si>
+    <t>Looked for ways to implement Time Series Map Chart. Committed to repo.</t>
+  </si>
+  <si>
+    <t>looked for ways to deploy tableau. Currently most reasonable option is through Tableau public and embed unto a website.</t>
+  </si>
+  <si>
+    <t>Adjusted misinterpreted data on Covid Death/Infection Report. Started on a Time Series Map Chart Dashboard.</t>
+  </si>
+  <si>
+    <t>Finished Time Series Dashboard. Started on Reworking Political Affiliations Dashboard</t>
+  </si>
+  <si>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>Updates to Jira Project Management Board</t>
+  </si>
+  <si>
+    <t>Demo Recording</t>
+  </si>
+  <si>
+    <t>created a baseline script to use to record 2nd demo</t>
+  </si>
+  <si>
+    <t>Demo Recorded</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Emailed Supervisor regarding missing interim evaulation report</t>
+  </si>
+  <si>
+    <t>Took some inspirations from other dashboards on Tableau Public for data visualization. Changed overall color theme of dashboards to black to help dashboard visualization. Adjusted dashboard heights, widiths, and inner/outer paddings to ensure visualization consistency.</t>
+  </si>
 </sst>
 </file>
 
@@ -349,7 +392,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border/>
     <border>
       <left style="thin">
@@ -519,11 +562,53 @@
         <color rgb="FF284E3F"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -704,6 +789,30 @@
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,7 +857,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="4">
+  <tableStyles count="5">
     <tableStyle count="3" pivot="0" name="94 - 916-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -765,6 +874,11 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="1015 - 1028-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="1029 - 1112-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -786,6 +900,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -839,6 +957,19 @@
     <tableColumn name="Challenges/ Results" id="5"/>
   </tableColumns>
   <tableStyleInfo name="1015 - 1028-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E16" displayName="Table2_2" name="Table2_2" id="5">
+  <tableColumns count="5">
+    <tableColumn name="DATE" id="1"/>
+    <tableColumn name="Duration (hours)" id="2"/>
+    <tableColumn name="Type" id="3"/>
+    <tableColumn name="Description" id="4"/>
+    <tableColumn name="Challenges/ Results" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="1029 - 1112-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -2055,4 +2186,237 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="12.75"/>
+    <col customWidth="1" min="2" max="2" width="17.5"/>
+    <col customWidth="1" min="3" max="3" width="15.75"/>
+    <col customWidth="1" min="4" max="4" width="17.0"/>
+    <col customWidth="1" min="5" max="5" width="23.25"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="35">
+        <v>45599.0</v>
+      </c>
+      <c r="B2" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="29">
+        <v>45599.0</v>
+      </c>
+      <c r="B3" s="30">
+        <v>6.0</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="G3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="34">
+        <f>SUM(Table2_2[Duration (hours)])</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="25">
+        <v>45600.0</v>
+      </c>
+      <c r="B4" s="26">
+        <v>2.0</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="61"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="39">
+        <v>45602.0</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="62"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="35">
+        <v>45603.0</v>
+      </c>
+      <c r="B6" s="36">
+        <v>8.0</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="53"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="39">
+        <v>45605.0</v>
+      </c>
+      <c r="B7" s="16">
+        <v>7.0</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="62"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="25">
+        <v>45606.0</v>
+      </c>
+      <c r="B8" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="64"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="29">
+        <v>45606.0</v>
+      </c>
+      <c r="B9" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="35">
+        <v>45606.0</v>
+      </c>
+      <c r="B10" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="53"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="39">
+        <v>45606.0</v>
+      </c>
+      <c r="B11" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="35"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="65"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="43"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="25"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="46"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="29"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="43"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="66"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68"/>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A16">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>